<commit_message>
completed unit testing according to test plan. 8 test passed
</commit_message>
<xml_diff>
--- a/tests/A02_pixell_test_plan_chequing_account.xlsx
+++ b/tests/A02_pixell_test_plan_chequing_account.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Intermediate Software Development0315\2. Assignments\assignments\assignment_02\instructions\given_files\assignment_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ralph\OneDrive - Red River College Polytech\Desktop\Intermidiate_Software_Development\Project\Vitug_Ralph_Assignment_1\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2873F10E-F8B1-4F89-8CDF-A98B96DD770E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0E3B22-A3A6-4869-86EA-8D111C461A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="3555" windowWidth="25185" windowHeight="11415" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="34">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -249,12 +249,54 @@
   </si>
   <si>
     <t>Attributes are set to input values (ensure to test for superclass and subclass attributes)</t>
+  </si>
+  <si>
+    <t>Ralph Vitug</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>account_number=2121, client_number=2222, balance=1000.0, date_created=valid date, overdraft_limit=-100.0, overdraft_rate=0.05</t>
+  </si>
+  <si>
+    <t>Object created</t>
+  </si>
+  <si>
+    <t>overdraft_limit = "not_Mark"</t>
+  </si>
+  <si>
+    <t>overdraft_limit=-100.0 overdraft_fee=0.05</t>
+  </si>
+  <si>
+    <t>BASE_SERVICE_CHARGE=0.50</t>
+  </si>
+  <si>
+    <t>balance=-600.00</t>
+  </si>
+  <si>
+    <t>balance=50.00</t>
+  </si>
+  <si>
+    <t>balance=-100.00</t>
+  </si>
+  <si>
+    <t>date_created="not_Mark"</t>
+  </si>
+  <si>
+    <t>"Account Number: 2121 Balance: $1,000.00 "
+ "Overdraft Limit: $-100.00 "
+ "Overdraft Rate: %5.00 "
+  "Account Type: Chequing"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -555,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -584,6 +626,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="8" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1154,53 +1205,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="B1:G32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
-    <col min="7" max="7" width="48.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="4" max="4" width="32.7265625" customWidth="1"/>
+    <col min="5" max="5" width="31.54296875" customWidth="1"/>
+    <col min="6" max="6" width="28.26953125" customWidth="1"/>
+    <col min="7" max="7" width="48.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="2.15">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-    </row>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+    </row>
+    <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
-    </row>
-    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="20"/>
+    </row>
+    <row r="4" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="19"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="8" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +1273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="11">
         <v>1</v>
       </c>
@@ -1230,11 +1283,17 @@
       <c r="D7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="3">
         <v>2</v>
       </c>
@@ -1244,11 +1303,17 @@
       <c r="D8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="12">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="11">
         <v>3</v>
       </c>
@@ -1258,11 +1323,17 @@
       <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="11">
         <v>4</v>
       </c>
@@ -1272,11 +1343,17 @@
       <c r="D10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="16">
+        <v>45931</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="3">
         <v>5</v>
       </c>
@@ -1286,11 +1363,17 @@
       <c r="D11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="11">
         <v>6</v>
       </c>
@@ -1300,11 +1383,17 @@
       <c r="D12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="15">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="11">
         <v>7</v>
       </c>
@@ -1314,11 +1403,17 @@
       <c r="D13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="2:7" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="3">
         <v>8</v>
       </c>
@@ -1328,11 +1423,17 @@
       <c r="D14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="11">
         <v>9</v>
       </c>
@@ -1342,7 +1443,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="11">
         <v>10</v>
       </c>
@@ -1352,7 +1453,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="3">
         <v>11</v>
       </c>
@@ -1362,7 +1463,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="11">
         <v>12</v>
       </c>
@@ -1372,7 +1473,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="11">
         <v>13</v>
       </c>
@@ -1382,7 +1483,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="3">
         <v>14</v>
       </c>
@@ -1392,7 +1493,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="11">
         <v>15</v>
       </c>
@@ -1402,7 +1503,7 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="11">
         <v>16</v>
       </c>
@@ -1412,7 +1513,7 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="3">
         <v>17</v>
       </c>
@@ -1422,7 +1523,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="11">
         <v>18</v>
       </c>
@@ -1432,7 +1533,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="11">
         <v>19</v>
       </c>
@@ -1442,7 +1543,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="3">
         <v>20</v>
       </c>
@@ -1452,7 +1553,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="11">
         <v>21</v>
       </c>
@@ -1462,7 +1563,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="11">
         <v>22</v>
       </c>
@@ -1472,7 +1573,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B29" s="3">
         <v>23</v>
       </c>
@@ -1482,7 +1583,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B30" s="11">
         <v>24</v>
       </c>
@@ -1492,15 +1593,15 @@
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="20" t="s">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B32" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>